<commit_message>
advancedCheckout - Guest profile with images
</commit_message>
<xml_diff>
--- a/scripts/csv/b2bProductVariation.xlsx
+++ b/scripts/csv/b2bProductVariation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cpd\SFDC\Treinamentos\b2bSimpleTemplate\scripts\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB5E3E8-F503-4CA7-ACC7-95BF6A9A93A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AA841E-0AD5-44D7-B882-340250D6D439}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4485,9 +4485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F67779-B206-4BE8-BB96-D19EC851461B}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
-    </sheetView>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
advancedCheckout - fixing csv
</commit_message>
<xml_diff>
--- a/scripts/csv/b2bProductVariation.xlsx
+++ b/scripts/csv/b2bProductVariation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cpd\SFDC\Treinamentos\b2bSimpleTemplate\scripts\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AA841E-0AD5-44D7-B882-340250D6D439}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E35BCE4-6A6B-46EE-A944-AC990974F821}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4485,7 +4485,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F67779-B206-4BE8-BB96-D19EC851461B}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
advancedCheckout - Guest profile with menu
</commit_message>
<xml_diff>
--- a/scripts/csv/b2bProductVariation.xlsx
+++ b/scripts/csv/b2bProductVariation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cpd\SFDC\Treinamentos\b2bSimpleTemplate\scripts\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E35BCE4-6A6B-46EE-A944-AC990974F821}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8374B9EC-4730-43F1-BEE7-A7FA1843FA06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="221">
   <si>
     <t>Product Name</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>https://thumbs2.imgbox.com/8f/40/eFukFf5X_t.png</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1545,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAAB22D-FBC4-4D9B-B04E-EFAFF7DF6BA7}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1680,7 +1685,7 @@
         <v>168</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H3" t="s">
         <v>171</v>
@@ -2130,7 +2135,7 @@
         <v>168</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H12" t="s">
         <v>171</v>
@@ -2730,7 +2735,7 @@
         <v>168</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H24" t="s">
         <v>171</v>
@@ -3480,7 +3485,7 @@
         <v>168</v>
       </c>
       <c r="G39" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H39" t="s">
         <v>171</v>

</xml_diff>